<commit_message>
Finished c284130850 (not tested)
</commit_message>
<xml_diff>
--- a/完成度统计.xlsx
+++ b/完成度统计.xlsx
@@ -78,10 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -147,6 +143,10 @@
   </si>
   <si>
     <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,8 +480,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1">
         <f>COUNTA(A:A)</f>
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "=c")</f>
@@ -527,11 +527,11 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <f>COUNTIF(B:B, "=I")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -542,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <f>COUNTIF(B:B, "=n")</f>
@@ -557,11 +557,11 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <f>SUM(F6:F8)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -572,11 +572,11 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <f>COUNTIF(B:B, "=w")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <f>COUNTIF(B:B, "=r")</f>
@@ -602,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <f>COUNTIF(B:B, "=d")</f>
@@ -734,7 +734,7 @@
         <v>284130834</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -742,7 +742,7 @@
         <v>284130835</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>284130850</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -870,7 +870,7 @@
         <v>284130851</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>284130852</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
         <v>284130853</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -910,7 +910,7 @@
         <v>284130856</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
         <v>284130857</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>284130858</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>284130859</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>284130861</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>284130862</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>284130863</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>284130865</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -990,7 +990,7 @@
         <v>284130866</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -998,7 +998,7 @@
         <v>284130867</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>284130868</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1014,7 +1014,7 @@
         <v>284130869</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix (c284130843): fix c284130843
</commit_message>
<xml_diff>
--- a/完成度统计.xlsx
+++ b/完成度统计.xlsx
@@ -58,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,6 +135,10 @@
   </si>
   <si>
     <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1">
         <f>COUNTA(A:A)</f>
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "=c")</f>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <f>COUNTIF(B:B, "=I")</f>
@@ -538,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <f>COUNTIF(B:B, "=n")</f>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <f>SUM(F6:F8)</f>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <f>COUNTIF(B:B, "=t")</f>
@@ -583,11 +583,11 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <f>COUNTIF(B:B, "=r")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -598,11 +598,11 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <f>COUNTIF(B:B, "=d")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>284130834</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>284130835</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>284130836</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>284130838</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -802,7 +802,7 @@
         <v>284130843</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -826,7 +826,7 @@
         <v>284130846</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -834,7 +834,7 @@
         <v>284130847</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>284130848</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -850,7 +850,7 @@
         <v>284130849</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
         <v>284130850</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -866,7 +866,7 @@
         <v>284130851</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -874,7 +874,7 @@
         <v>284130852</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -882,7 +882,7 @@
         <v>284130853</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -906,7 +906,7 @@
         <v>284130856</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -914,7 +914,7 @@
         <v>284130857</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -922,7 +922,7 @@
         <v>284130858</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -930,7 +930,7 @@
         <v>284130859</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -946,7 +946,7 @@
         <v>284130861</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>284130862</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -962,7 +962,7 @@
         <v>284130863</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -978,7 +978,7 @@
         <v>284130865</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>284130866</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -994,7 +994,7 @@
         <v>284130867</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1002,7 +1002,7 @@
         <v>284130868</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
         <v>284130869</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix (c284130845): fix c2841030845
</commit_message>
<xml_diff>
--- a/完成度统计.xlsx
+++ b/完成度统计.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>c</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,10 @@
   </si>
   <si>
     <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -476,8 +480,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -587,7 +591,7 @@
       </c>
       <c r="F7">
         <f>COUNTIF(B:B, "=r")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -602,7 +606,7 @@
       </c>
       <c r="F8">
         <f>COUNTIF(B:B, "=d")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -818,7 +822,7 @@
         <v>284130845</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>